<commit_message>
Updated the description for kubelet
</commit_message>
<xml_diff>
--- a/tools/kubernetes-certs-checker.xlsx
+++ b/tools/kubernetes-certs-checker.xlsx
@@ -1,16 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24729"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mushegh.davtyan\kubernetes-the-hard-way\tools\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\New folder (3)\kubernetes-the-hard-way\tools\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A0D1D50-DC10-49B6-87B7-781BB565E523}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9336" tabRatio="500" activeTab="1"/>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9336" activeTab="1"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF01000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Information" sheetId="1" r:id="rId1"/>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="88">
   <si>
     <r>
       <rPr>
@@ -401,11 +402,17 @@
     <t>CA Server root certificate key for ETCD Server.
  (This could be the same as kube-api server or a separate one of its own.)</t>
   </si>
+  <si>
+    <t>Client Certificate for Kube-API Server to connect to Kubelet</t>
+  </si>
+  <si>
+    <t>Client Key for Kube-API Server to connect to Kubelet</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -938,7 +945,34 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="6" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="9" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="13" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="8" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="12" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="9" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="7" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="8" borderId="3" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -953,22 +987,19 @@
     <xf numFmtId="0" fontId="10" fillId="7" borderId="12" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="8" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="6" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="12" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="3" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="6" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="7" borderId="8" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="7" borderId="12" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="9" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="13" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="9" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -989,37 +1020,13 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="13" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="9" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="7" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="6" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="3" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="7">
-    <cellStyle name="Excel Built-in 20% - Accent2" xfId="3"/>
-    <cellStyle name="Excel Built-in 20% - Accent3" xfId="6"/>
-    <cellStyle name="Excel Built-in 20% - Accent5" xfId="4"/>
-    <cellStyle name="Excel Built-in 40% - Accent5" xfId="5"/>
-    <cellStyle name="Excel Built-in Accent1" xfId="2"/>
+    <cellStyle name="Excel Built-in 20% - Accent2" xfId="3" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
+    <cellStyle name="Excel Built-in 20% - Accent3" xfId="6" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
+    <cellStyle name="Excel Built-in 20% - Accent5" xfId="4" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
+    <cellStyle name="Excel Built-in 40% - Accent5" xfId="5" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
+    <cellStyle name="Excel Built-in Accent1" xfId="2" xr:uid="{00000000-0005-0000-0000-000004000000}"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -1123,6 +1130,11 @@
       <xdr:nvPicPr>
         <xdr:cNvPr id="2" name="Picture 2">
           <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+            </a:ext>
+          </a:extLst>
         </xdr:cNvPr>
         <xdr:cNvPicPr/>
       </xdr:nvPicPr>
@@ -1410,7 +1422,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L20"/>
   <sheetViews>
     <sheetView view="pageLayout" zoomScaleNormal="100" zoomScaleSheetLayoutView="130" workbookViewId="0">
@@ -1420,13 +1432,13 @@
       <selection sqref="A1:L17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="12.77734375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="35.109375" customWidth="1"/>
+    <col min="1" max="1" width="12.81640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="35.08984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" ht="14.4" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="38" t="s">
         <v>0</v>
       </c>
@@ -1442,7 +1454,7 @@
       <c r="K1" s="38"/>
       <c r="L1" s="38"/>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A2" s="38"/>
       <c r="B2" s="38"/>
       <c r="C2" s="38"/>
@@ -1456,7 +1468,7 @@
       <c r="K2" s="38"/>
       <c r="L2" s="38"/>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A3" s="38"/>
       <c r="B3" s="38"/>
       <c r="C3" s="38"/>
@@ -1470,7 +1482,7 @@
       <c r="K3" s="38"/>
       <c r="L3" s="38"/>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A4" s="38"/>
       <c r="B4" s="38"/>
       <c r="C4" s="38"/>
@@ -1484,7 +1496,7 @@
       <c r="K4" s="38"/>
       <c r="L4" s="38"/>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A5" s="38"/>
       <c r="B5" s="38"/>
       <c r="C5" s="38"/>
@@ -1498,7 +1510,7 @@
       <c r="K5" s="38"/>
       <c r="L5" s="38"/>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A6" s="38"/>
       <c r="B6" s="38"/>
       <c r="C6" s="38"/>
@@ -1512,7 +1524,7 @@
       <c r="K6" s="38"/>
       <c r="L6" s="38"/>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A7" s="38"/>
       <c r="B7" s="38"/>
       <c r="C7" s="38"/>
@@ -1526,7 +1538,7 @@
       <c r="K7" s="38"/>
       <c r="L7" s="38"/>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A8" s="38"/>
       <c r="B8" s="38"/>
       <c r="C8" s="38"/>
@@ -1540,7 +1552,7 @@
       <c r="K8" s="38"/>
       <c r="L8" s="38"/>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A9" s="38"/>
       <c r="B9" s="38"/>
       <c r="C9" s="38"/>
@@ -1554,7 +1566,7 @@
       <c r="K9" s="38"/>
       <c r="L9" s="38"/>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A10" s="38"/>
       <c r="B10" s="38"/>
       <c r="C10" s="38"/>
@@ -1568,7 +1580,7 @@
       <c r="K10" s="38"/>
       <c r="L10" s="38"/>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A11" s="38"/>
       <c r="B11" s="38"/>
       <c r="C11" s="38"/>
@@ -1582,7 +1594,7 @@
       <c r="K11" s="38"/>
       <c r="L11" s="38"/>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A12" s="38"/>
       <c r="B12" s="38"/>
       <c r="C12" s="38"/>
@@ -1596,7 +1608,7 @@
       <c r="K12" s="38"/>
       <c r="L12" s="38"/>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A13" s="38"/>
       <c r="B13" s="38"/>
       <c r="C13" s="38"/>
@@ -1610,7 +1622,7 @@
       <c r="K13" s="38"/>
       <c r="L13" s="38"/>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A14" s="38"/>
       <c r="B14" s="38"/>
       <c r="C14" s="38"/>
@@ -1624,7 +1636,7 @@
       <c r="K14" s="38"/>
       <c r="L14" s="38"/>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A15" s="38"/>
       <c r="B15" s="38"/>
       <c r="C15" s="38"/>
@@ -1638,7 +1650,7 @@
       <c r="K15" s="38"/>
       <c r="L15" s="38"/>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A16" s="38"/>
       <c r="B16" s="38"/>
       <c r="C16" s="38"/>
@@ -1652,7 +1664,7 @@
       <c r="K16" s="38"/>
       <c r="L16" s="38"/>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A17" s="38"/>
       <c r="B17" s="38"/>
       <c r="C17" s="38"/>
@@ -1666,7 +1678,7 @@
       <c r="K17" s="38"/>
       <c r="L17" s="38"/>
     </row>
-    <row r="18" spans="1:12" ht="25.8" x14ac:dyDescent="0.5">
+    <row r="18" spans="1:12" ht="26" x14ac:dyDescent="0.6">
       <c r="A18" s="2" t="s">
         <v>1</v>
       </c>
@@ -1684,7 +1696,7 @@
       <c r="K18" s="42"/>
       <c r="L18" s="42"/>
     </row>
-    <row r="19" spans="1:12" ht="25.8" x14ac:dyDescent="0.5">
+    <row r="19" spans="1:12" ht="26" x14ac:dyDescent="0.6">
       <c r="A19" s="1" t="s">
         <v>3</v>
       </c>
@@ -1702,7 +1714,7 @@
       <c r="K19" s="44"/>
       <c r="L19" s="44"/>
     </row>
-    <row r="20" spans="1:12" ht="25.8" x14ac:dyDescent="0.5">
+    <row r="20" spans="1:12" ht="26" x14ac:dyDescent="0.6">
       <c r="A20" s="1" t="s">
         <v>82</v>
       </c>
@@ -1729,8 +1741,8 @@
     <mergeCell ref="E18:L20"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="B19" r:id="rId1"/>
-    <hyperlink ref="B20" r:id="rId2"/>
+    <hyperlink ref="B19" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="B20" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="6.1416666666666668E-2" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup scale="67" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId3"/>
@@ -1739,7 +1751,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AME24"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
@@ -1748,29 +1760,29 @@
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
       <selection pane="bottomRight" sqref="A1:XFD1"/>
     </sheetView>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="1">
-      <pane xSplit="1" topLeftCell="E1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="G4" sqref="G4"/>
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="85" zoomScaleNormal="85" workbookViewId="1">
+      <pane xSplit="1" topLeftCell="F1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="J25" sqref="J25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="32.109375" style="10" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.21875" style="8" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="32.08984375" style="10" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.1796875" style="8" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="54" style="8" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="26.109375" style="8" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="35.77734375" style="8" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.44140625" style="8" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.33203125" style="8" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="24.6640625" style="8" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.77734375" style="8" customWidth="1"/>
-    <col min="10" max="10" width="34.44140625" style="8" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="64.77734375" style="8" bestFit="1" customWidth="1"/>
-    <col min="12" max="1019" width="8.88671875" style="8"/>
-    <col min="1020" max="16384" width="8.88671875" style="9"/>
+    <col min="4" max="4" width="26.08984375" style="8" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="35.81640625" style="8" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.453125" style="8" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.36328125" style="8" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="24.6328125" style="8" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.81640625" style="8" customWidth="1"/>
+    <col min="10" max="10" width="34.453125" style="8" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="64.81640625" style="8" bestFit="1" customWidth="1"/>
+    <col min="12" max="1019" width="8.90625" style="8"/>
+    <col min="1020" max="16384" width="8.90625" style="9"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1019" s="3" customFormat="1" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:1019" s="3" customFormat="1" ht="19" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="12" t="s">
         <v>6</v>
       </c>
@@ -1805,11 +1817,11 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:1019" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="50" t="s">
+    <row r="2" spans="1:1019" s="5" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="51" t="s">
         <v>17</v>
       </c>
-      <c r="B2" s="54" t="s">
+      <c r="B2" s="49" t="s">
         <v>18</v>
       </c>
       <c r="C2" s="13" t="s">
@@ -2842,9 +2854,9 @@
       <c r="AMD2" s="4"/>
       <c r="AME2" s="4"/>
     </row>
-    <row r="3" spans="1:1019" s="5" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="51"/>
-      <c r="B3" s="55"/>
+    <row r="3" spans="1:1019" s="5" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A3" s="52"/>
+      <c r="B3" s="50"/>
       <c r="C3" s="15" t="s">
         <v>24</v>
       </c>
@@ -3869,11 +3881,11 @@
       <c r="AMD3" s="4"/>
       <c r="AME3" s="4"/>
     </row>
-    <row r="4" spans="1:1019" s="6" customFormat="1" ht="100.8" x14ac:dyDescent="0.3">
-      <c r="A4" s="47" t="s">
+    <row r="4" spans="1:1019" s="6" customFormat="1" ht="101.5" x14ac:dyDescent="0.35">
+      <c r="A4" s="56" t="s">
         <v>27</v>
       </c>
-      <c r="B4" s="66" t="s">
+      <c r="B4" s="53" t="s">
         <v>18</v>
       </c>
       <c r="C4" s="28" t="s">
@@ -3902,9 +3914,9 @@
         <v>32</v>
       </c>
     </row>
-    <row r="5" spans="1:1019" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="48"/>
-      <c r="B5" s="67"/>
+    <row r="5" spans="1:1019" s="6" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="57"/>
+      <c r="B5" s="54"/>
       <c r="C5" s="31" t="s">
         <v>33</v>
       </c>
@@ -3923,9 +3935,9 @@
         <v>35</v>
       </c>
     </row>
-    <row r="6" spans="1:1019" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="48"/>
-      <c r="B6" s="46"/>
+    <row r="6" spans="1:1019" s="6" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="57"/>
+      <c r="B6" s="55"/>
       <c r="C6" s="31" t="s">
         <v>19</v>
       </c>
@@ -3934,13 +3946,13 @@
       </c>
       <c r="E6" s="31"/>
       <c r="F6" s="31"/>
-      <c r="G6" s="45" t="s">
+      <c r="G6" s="61" t="s">
         <v>20</v>
       </c>
       <c r="H6" s="31" t="s">
         <v>36</v>
       </c>
-      <c r="I6" s="45" t="s">
+      <c r="I6" s="61" t="s">
         <v>22</v>
       </c>
       <c r="J6" s="31" t="s">
@@ -3950,9 +3962,9 @@
         <v>38</v>
       </c>
     </row>
-    <row r="7" spans="1:1019" s="7" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="48"/>
-      <c r="B7" s="68" t="s">
+    <row r="7" spans="1:1019" s="7" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="57"/>
+      <c r="B7" s="59" t="s">
         <v>39</v>
       </c>
       <c r="C7" s="33" t="s">
@@ -3965,21 +3977,21 @@
       <c r="F7" s="33" t="s">
         <v>42</v>
       </c>
-      <c r="G7" s="46"/>
+      <c r="G7" s="55"/>
       <c r="H7" s="33" t="s">
         <v>30</v>
       </c>
-      <c r="I7" s="46"/>
+      <c r="I7" s="55"/>
       <c r="J7" s="33" t="s">
         <v>43</v>
       </c>
       <c r="K7" s="34" t="s">
-        <v>44</v>
+        <v>86</v>
       </c>
     </row>
-    <row r="8" spans="1:1019" s="7" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="48"/>
-      <c r="B8" s="69"/>
+    <row r="8" spans="1:1019" s="7" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="57"/>
+      <c r="B8" s="60"/>
       <c r="C8" s="33" t="s">
         <v>45</v>
       </c>
@@ -3995,12 +4007,12 @@
         <v>46</v>
       </c>
       <c r="K8" s="34" t="s">
-        <v>47</v>
+        <v>87</v>
       </c>
     </row>
-    <row r="9" spans="1:1019" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="48"/>
-      <c r="B9" s="45" t="s">
+    <row r="9" spans="1:1019" s="6" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="57"/>
+      <c r="B9" s="61" t="s">
         <v>48</v>
       </c>
       <c r="C9" s="31" t="s">
@@ -4029,9 +4041,9 @@
         <v>44</v>
       </c>
     </row>
-    <row r="10" spans="1:1019" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="48"/>
-      <c r="B10" s="46"/>
+    <row r="10" spans="1:1019" s="6" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="57"/>
+      <c r="B10" s="55"/>
       <c r="C10" s="31" t="s">
         <v>53</v>
       </c>
@@ -4050,8 +4062,8 @@
         <v>47</v>
       </c>
     </row>
-    <row r="11" spans="1:1019" s="6" customFormat="1" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="49"/>
+    <row r="11" spans="1:1019" s="6" customFormat="1" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A11" s="58"/>
       <c r="B11" s="35" t="s">
         <v>48</v>
       </c>
@@ -4079,11 +4091,11 @@
         <v>83</v>
       </c>
     </row>
-    <row r="12" spans="1:1019" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="47" t="s">
+    <row r="12" spans="1:1019" s="6" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="56" t="s">
         <v>58</v>
       </c>
-      <c r="B12" s="58" t="s">
+      <c r="B12" s="66" t="s">
         <v>18</v>
       </c>
       <c r="C12" s="17" t="s">
@@ -4102,9 +4114,9 @@
       <c r="J12" s="17"/>
       <c r="K12" s="18"/>
     </row>
-    <row r="13" spans="1:1019" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="48"/>
-      <c r="B13" s="59"/>
+    <row r="13" spans="1:1019" s="6" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="57"/>
+      <c r="B13" s="67"/>
       <c r="C13" s="11" t="s">
         <v>61</v>
       </c>
@@ -4119,9 +4131,9 @@
       <c r="J13" s="11"/>
       <c r="K13" s="19"/>
     </row>
-    <row r="14" spans="1:1019" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="48"/>
-      <c r="B14" s="60" t="s">
+    <row r="14" spans="1:1019" s="6" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="57"/>
+      <c r="B14" s="68" t="s">
         <v>62</v>
       </c>
       <c r="C14" s="11" t="s">
@@ -4146,9 +4158,9 @@
       <c r="J14" s="11"/>
       <c r="K14" s="19"/>
     </row>
-    <row r="15" spans="1:1019" s="6" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="49"/>
-      <c r="B15" s="61"/>
+    <row r="15" spans="1:1019" s="6" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A15" s="58"/>
+      <c r="B15" s="69"/>
       <c r="C15" s="20"/>
       <c r="D15" s="20"/>
       <c r="E15" s="20"/>
@@ -4161,11 +4173,11 @@
       <c r="J15" s="20"/>
       <c r="K15" s="22"/>
     </row>
-    <row r="16" spans="1:1019" s="5" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A16" s="50" t="s">
+    <row r="16" spans="1:1019" s="5" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+      <c r="A16" s="51" t="s">
         <v>67</v>
       </c>
-      <c r="B16" s="54" t="s">
+      <c r="B16" s="49" t="s">
         <v>18</v>
       </c>
       <c r="C16" s="13" t="s">
@@ -5200,9 +5212,9 @@
       <c r="AMD16" s="4"/>
       <c r="AME16" s="4"/>
     </row>
-    <row r="17" spans="1:1019" s="5" customFormat="1" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="51"/>
-      <c r="B17" s="55"/>
+    <row r="17" spans="1:1019" s="5" customFormat="1" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A17" s="52"/>
+      <c r="B17" s="50"/>
       <c r="C17" s="15" t="s">
         <v>70</v>
       </c>
@@ -6229,17 +6241,17 @@
       <c r="AMD17" s="4"/>
       <c r="AME17" s="4"/>
     </row>
-    <row r="18" spans="1:1019" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="52" t="s">
+    <row r="18" spans="1:1019" s="5" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="62" t="s">
         <v>72</v>
       </c>
-      <c r="B18" s="56" t="s">
+      <c r="B18" s="64" t="s">
         <v>18</v>
       </c>
       <c r="C18" s="13" t="s">
         <v>73</v>
       </c>
-      <c r="D18" s="56" t="s">
+      <c r="D18" s="64" t="s">
         <v>74</v>
       </c>
       <c r="E18" s="23"/>
@@ -7266,13 +7278,13 @@
       <c r="AMD18" s="4"/>
       <c r="AME18" s="4"/>
     </row>
-    <row r="19" spans="1:1019" s="5" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="53"/>
-      <c r="B19" s="57"/>
+    <row r="19" spans="1:1019" s="5" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A19" s="63"/>
+      <c r="B19" s="65"/>
       <c r="C19" s="15" t="s">
         <v>78</v>
       </c>
-      <c r="D19" s="57"/>
+      <c r="D19" s="65"/>
       <c r="E19" s="25"/>
       <c r="F19" s="25"/>
       <c r="G19" s="25"/>
@@ -8297,75 +8309,76 @@
       <c r="AMD19" s="4"/>
       <c r="AME19" s="4"/>
     </row>
-    <row r="20" spans="1:1019" x14ac:dyDescent="0.3">
-      <c r="A20" s="62" t="s">
+    <row r="20" spans="1:1019" x14ac:dyDescent="0.35">
+      <c r="A20" s="45" t="s">
         <v>81</v>
       </c>
-      <c r="B20" s="63"/>
-      <c r="C20" s="63"/>
-      <c r="D20" s="63"/>
-      <c r="E20" s="63"/>
-      <c r="F20" s="63"/>
-      <c r="G20" s="63"/>
-      <c r="H20" s="63"/>
-      <c r="I20" s="63"/>
-      <c r="J20" s="63"/>
-      <c r="K20" s="63"/>
+      <c r="B20" s="46"/>
+      <c r="C20" s="46"/>
+      <c r="D20" s="46"/>
+      <c r="E20" s="46"/>
+      <c r="F20" s="46"/>
+      <c r="G20" s="46"/>
+      <c r="H20" s="46"/>
+      <c r="I20" s="46"/>
+      <c r="J20" s="46"/>
+      <c r="K20" s="46"/>
     </row>
-    <row r="21" spans="1:1019" x14ac:dyDescent="0.3">
-      <c r="A21" s="64"/>
-      <c r="B21" s="65"/>
-      <c r="C21" s="65"/>
-      <c r="D21" s="65"/>
-      <c r="E21" s="65"/>
-      <c r="F21" s="65"/>
-      <c r="G21" s="65"/>
-      <c r="H21" s="65"/>
-      <c r="I21" s="65"/>
-      <c r="J21" s="65"/>
-      <c r="K21" s="65"/>
+    <row r="21" spans="1:1019" x14ac:dyDescent="0.35">
+      <c r="A21" s="47"/>
+      <c r="B21" s="48"/>
+      <c r="C21" s="48"/>
+      <c r="D21" s="48"/>
+      <c r="E21" s="48"/>
+      <c r="F21" s="48"/>
+      <c r="G21" s="48"/>
+      <c r="H21" s="48"/>
+      <c r="I21" s="48"/>
+      <c r="J21" s="48"/>
+      <c r="K21" s="48"/>
     </row>
-    <row r="22" spans="1:1019" x14ac:dyDescent="0.3">
-      <c r="A22" s="64"/>
-      <c r="B22" s="65"/>
-      <c r="C22" s="65"/>
-      <c r="D22" s="65"/>
-      <c r="E22" s="65"/>
-      <c r="F22" s="65"/>
-      <c r="G22" s="65"/>
-      <c r="H22" s="65"/>
-      <c r="I22" s="65"/>
-      <c r="J22" s="65"/>
-      <c r="K22" s="65"/>
+    <row r="22" spans="1:1019" x14ac:dyDescent="0.35">
+      <c r="A22" s="47"/>
+      <c r="B22" s="48"/>
+      <c r="C22" s="48"/>
+      <c r="D22" s="48"/>
+      <c r="E22" s="48"/>
+      <c r="F22" s="48"/>
+      <c r="G22" s="48"/>
+      <c r="H22" s="48"/>
+      <c r="I22" s="48"/>
+      <c r="J22" s="48"/>
+      <c r="K22" s="48"/>
     </row>
-    <row r="23" spans="1:1019" x14ac:dyDescent="0.3">
-      <c r="A23" s="64"/>
-      <c r="B23" s="65"/>
-      <c r="C23" s="65"/>
-      <c r="D23" s="65"/>
-      <c r="E23" s="65"/>
-      <c r="F23" s="65"/>
-      <c r="G23" s="65"/>
-      <c r="H23" s="65"/>
-      <c r="I23" s="65"/>
-      <c r="J23" s="65"/>
-      <c r="K23" s="65"/>
+    <row r="23" spans="1:1019" x14ac:dyDescent="0.35">
+      <c r="A23" s="47"/>
+      <c r="B23" s="48"/>
+      <c r="C23" s="48"/>
+      <c r="D23" s="48"/>
+      <c r="E23" s="48"/>
+      <c r="F23" s="48"/>
+      <c r="G23" s="48"/>
+      <c r="H23" s="48"/>
+      <c r="I23" s="48"/>
+      <c r="J23" s="48"/>
+      <c r="K23" s="48"/>
     </row>
-    <row r="24" spans="1:1019" x14ac:dyDescent="0.3">
-      <c r="A24" s="64"/>
-      <c r="B24" s="65"/>
-      <c r="C24" s="65"/>
-      <c r="D24" s="65"/>
-      <c r="E24" s="65"/>
-      <c r="F24" s="65"/>
-      <c r="G24" s="65"/>
-      <c r="H24" s="65"/>
-      <c r="I24" s="65"/>
-      <c r="J24" s="65"/>
-      <c r="K24" s="65"/>
+    <row r="24" spans="1:1019" x14ac:dyDescent="0.35">
+      <c r="A24" s="47"/>
+      <c r="B24" s="48"/>
+      <c r="C24" s="48"/>
+      <c r="D24" s="48"/>
+      <c r="E24" s="48"/>
+      <c r="F24" s="48"/>
+      <c r="G24" s="48"/>
+      <c r="H24" s="48"/>
+      <c r="I24" s="48"/>
+      <c r="J24" s="48"/>
+      <c r="K24" s="48"/>
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="D18:D19"/>
     <mergeCell ref="A20:K24"/>
     <mergeCell ref="B2:B3"/>
     <mergeCell ref="A2:A3"/>
@@ -8382,10 +8395,9 @@
     <mergeCell ref="B18:B19"/>
     <mergeCell ref="B12:B13"/>
     <mergeCell ref="B14:B15"/>
-    <mergeCell ref="D18:D19"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="D12" r:id="rId1"/>
+    <hyperlink ref="D12" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>

</xml_diff>